<commit_message>
[T2] Final - sejeito a erros
</commit_message>
<xml_diff>
--- a/Trabalho 2/Planilhas/indicadoresResp.xlsx
+++ b/Trabalho 2/Planilhas/indicadoresResp.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9288"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9288" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Plan2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="34">
   <si>
     <t>[FILENAME]  [DISK NAME]  [DATE]  [INITIALS]</t>
   </si>
@@ -103,6 +102,21 @@
   </si>
   <si>
     <t>Idade</t>
+  </si>
+  <si>
+    <t>Homem</t>
+  </si>
+  <si>
+    <t>Mulher</t>
+  </si>
+  <si>
+    <t>Indices</t>
+  </si>
+  <si>
+    <t>Idade por Data de Nascimento</t>
+  </si>
+  <si>
+    <t>Ambos os sexos</t>
   </si>
 </sst>
 </file>
@@ -110,11 +124,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="General_)"/>
-    <numFmt numFmtId="169" formatCode="0.00_)"/>
-    <numFmt numFmtId="170" formatCode="0.0_)"/>
+    <numFmt numFmtId="164" formatCode="General_)"/>
+    <numFmt numFmtId="165" formatCode="0.00_)"/>
+    <numFmt numFmtId="166" formatCode="0.0_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +151,11 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,55 +176,77 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="fill"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,21 +551,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:F94"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -573,20 +618,20 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1043,530 +1088,530 @@
       <c r="E46" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="13"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="A50" s="12"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F52" s="11"/>
+      <c r="A52" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" s="10"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="15" t="s">
+      <c r="B54" s="10"/>
+      <c r="C54" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E54" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="11"/>
+      <c r="F54" s="10"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F55" s="11"/>
+      <c r="A55" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="10"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="17">
+      <c r="B58" s="10"/>
+      <c r="C58" s="16">
         <v>1.3004743991253267</v>
       </c>
-      <c r="D58" s="17">
+      <c r="D58" s="16">
         <v>1.2696484864187934</v>
       </c>
-      <c r="E58" s="17">
+      <c r="E58" s="16">
         <v>1.2862371231688223</v>
       </c>
-      <c r="F58" s="11"/>
+      <c r="F58" s="10"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="18">
+      <c r="B62" s="10"/>
+      <c r="C62" s="17">
         <v>14.356298493256622</v>
       </c>
-      <c r="D62" s="18">
+      <c r="D62" s="17">
         <v>12.877852481324528</v>
       </c>
-      <c r="E62" s="18">
+      <c r="E62" s="17">
         <v>13.666243121752602</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="18">
+      <c r="B64" s="10"/>
+      <c r="C64" s="17">
         <v>3.0758313760072902</v>
       </c>
-      <c r="D64" s="18">
+      <c r="D64" s="17">
         <v>2.7639996952772456</v>
       </c>
-      <c r="E64" s="18">
+      <c r="E64" s="17">
         <v>2.9302859015319083</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="13" t="s">
+      <c r="A65" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="18">
+      <c r="B65" s="10"/>
+      <c r="C65" s="17">
         <v>-2.2141459597587279</v>
       </c>
-      <c r="D65" s="18">
+      <c r="D65" s="17">
         <v>-2.2999248649286512</v>
       </c>
-      <c r="E65" s="18">
+      <c r="E65" s="17">
         <v>-2.2541827238992624</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="18">
+      <c r="B66" s="10"/>
+      <c r="C66" s="17">
         <v>1.5714413655282691</v>
       </c>
-      <c r="D66" s="18">
+      <c r="D66" s="17">
         <v>1.4359910435409979</v>
       </c>
-      <c r="E66" s="18">
+      <c r="E66" s="17">
         <v>1.508220780194133</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="18">
+      <c r="B67" s="10"/>
+      <c r="C67" s="17">
         <v>-0.12030282606720277</v>
       </c>
-      <c r="D67" s="18">
+      <c r="D67" s="17">
         <v>-0.34178241899079964</v>
       </c>
-      <c r="E67" s="18">
+      <c r="E67" s="17">
         <v>-0.22367703218766977</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="18">
+      <c r="B68" s="10"/>
+      <c r="C68" s="17">
         <v>-1.0274605271673369</v>
       </c>
-      <c r="D68" s="18">
+      <c r="D68" s="17">
         <v>-0.9692274830049854</v>
       </c>
-      <c r="E68" s="18">
+      <c r="E68" s="17">
         <v>-1.0002806202928554</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B69" s="11"/>
-      <c r="C69" s="18">
+      <c r="B69" s="10"/>
+      <c r="C69" s="17">
         <v>1.6941433187577104</v>
       </c>
-      <c r="D69" s="18">
+      <c r="D69" s="17">
         <v>1.6976194281668384</v>
       </c>
-      <c r="E69" s="18">
+      <c r="E69" s="17">
         <v>1.6957657709476077</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B70" s="11"/>
-      <c r="C70" s="18">
+      <c r="B70" s="10"/>
+      <c r="C70" s="17">
         <v>-0.71903867562950907</v>
       </c>
-      <c r="D70" s="18">
+      <c r="D70" s="17">
         <v>-0.50833431671150286</v>
       </c>
-      <c r="E70" s="18">
+      <c r="E70" s="17">
         <v>-0.62069374216746986</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B71" s="11"/>
-      <c r="C71" s="18">
+      <c r="B71" s="10"/>
+      <c r="C71" s="17">
         <v>-1.4248527347761648</v>
       </c>
-      <c r="D71" s="18">
+      <c r="D71" s="17">
         <v>-1.0311429642652818</v>
       </c>
-      <c r="E71" s="18">
+      <c r="E71" s="17">
         <v>-1.2410911771934128</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="13" t="s">
+      <c r="A72" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B72" s="11"/>
-      <c r="C72" s="18">
+      <c r="B72" s="10"/>
+      <c r="C72" s="17">
         <v>0.83673318633504223</v>
       </c>
-      <c r="D72" s="18">
+      <c r="D72" s="17">
         <v>0.54131607367718182</v>
       </c>
-      <c r="E72" s="18">
+      <c r="E72" s="17">
         <v>0.69884910820265311</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="13" t="s">
+      <c r="A73" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B73" s="11"/>
-      <c r="C73" s="18">
+      <c r="B73" s="10"/>
+      <c r="C73" s="17">
         <v>-1.6723485232293687</v>
       </c>
-      <c r="D73" s="18">
+      <c r="D73" s="17">
         <v>-1.288514192761042</v>
       </c>
-      <c r="E73" s="18">
+      <c r="E73" s="17">
         <v>-1.4931962651356301</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="13" t="s">
+      <c r="A75" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="13" t="s">
+      <c r="A77" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B77" s="11"/>
-      <c r="C77" s="18">
+      <c r="B77" s="10"/>
+      <c r="C77" s="17">
         <v>8.8822880714497696</v>
       </c>
-      <c r="D77" s="18">
+      <c r="D77" s="17">
         <v>7.9758369874411725</v>
       </c>
-      <c r="E77" s="18">
+      <c r="E77" s="17">
         <v>8.4561277597749136</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="13" t="s">
+      <c r="A79" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="18">
+      <c r="B79" s="10"/>
+      <c r="C79" s="17">
         <v>4.3200155952092274</v>
       </c>
-      <c r="D79" s="18">
+      <c r="D79" s="17">
         <v>3.8135502515252053</v>
       </c>
-      <c r="E79" s="18">
+      <c r="E79" s="17">
         <v>4.0817410701921801</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="13" t="s">
+      <c r="A80" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B80" s="11"/>
-      <c r="C80" s="18">
+      <c r="B80" s="10"/>
+      <c r="C80" s="17">
         <v>-2.8883756280043036</v>
       </c>
-      <c r="D80" s="18">
+      <c r="D80" s="17">
         <v>-2.9420074718701201</v>
       </c>
-      <c r="E80" s="18">
+      <c r="E80" s="17">
         <v>-2.9136955859097178</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="13" t="s">
+      <c r="A81" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B81" s="11"/>
-      <c r="C81" s="18">
+      <c r="B81" s="10"/>
+      <c r="C81" s="17">
         <v>1.6260544537265869</v>
       </c>
-      <c r="D81" s="18">
+      <c r="D81" s="17">
         <v>1.6365248428495107</v>
       </c>
-      <c r="E81" s="18">
+      <c r="E81" s="17">
         <v>1.6310095701244283</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="13" t="s">
+      <c r="A82" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B82" s="11"/>
-      <c r="C82" s="18">
+      <c r="B82" s="10"/>
+      <c r="C82" s="17">
         <v>-0.19547102010470496</v>
       </c>
-      <c r="D82" s="18">
+      <c r="D82" s="17">
         <v>-0.3985003814730419</v>
       </c>
-      <c r="E82" s="18">
+      <c r="E82" s="17">
         <v>-0.29026809221390693</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="13" t="s">
+      <c r="A83" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B83" s="11"/>
-      <c r="C83" s="18">
+      <c r="B83" s="10"/>
+      <c r="C83" s="17">
         <v>-1.2726272856422707</v>
       </c>
-      <c r="D83" s="18">
+      <c r="D83" s="17">
         <v>-1.1699767781350818</v>
       </c>
-      <c r="E83" s="18">
+      <c r="E83" s="17">
         <v>-1.2245161321740152</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="13" t="s">
+      <c r="A84" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B84" s="11"/>
-      <c r="C84" s="18">
+      <c r="B84" s="10"/>
+      <c r="C84" s="17">
         <v>2.3416111562801625</v>
       </c>
-      <c r="D84" s="18">
+      <c r="D84" s="17">
         <v>2.1845231724285554</v>
       </c>
-      <c r="E84" s="18">
+      <c r="E84" s="17">
         <v>2.2677066627054163</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B85" s="11"/>
-      <c r="C85" s="18">
+      <c r="B85" s="10"/>
+      <c r="C85" s="17">
         <v>-0.73958919388429933</v>
       </c>
-      <c r="D85" s="18">
+      <c r="D85" s="17">
         <v>-0.58180152638055738</v>
       </c>
-      <c r="E85" s="18">
+      <c r="E85" s="17">
         <v>-0.66509656392393701</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="13" t="s">
+      <c r="A86" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B86" s="11"/>
-      <c r="C86" s="18">
+      <c r="B86" s="10"/>
+      <c r="C86" s="17">
         <v>-1.6644539308400912</v>
       </c>
-      <c r="D86" s="18">
+      <c r="D86" s="17">
         <v>-1.3518920577904581</v>
       </c>
-      <c r="E86" s="18">
+      <c r="E86" s="17">
         <v>-1.5165338827592514</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="13" t="s">
+      <c r="A87" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B87" s="11"/>
-      <c r="C87" s="18">
+      <c r="B87" s="10"/>
+      <c r="C87" s="17">
         <v>0.73342567720065333</v>
       </c>
-      <c r="D87" s="18">
+      <c r="D87" s="17">
         <v>0.37303516120393887</v>
       </c>
-      <c r="E87" s="18">
+      <c r="E87" s="17">
         <v>0.5651546177727873</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="18">
+      <c r="B88" s="10"/>
+      <c r="C88" s="17">
         <v>-1.9829522020072403</v>
       </c>
-      <c r="D88" s="18">
+      <c r="D88" s="17">
         <v>-1.4998623312258754</v>
       </c>
-      <c r="E88" s="18">
+      <c r="E88" s="17">
         <v>-1.7565333417741869</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E89" s="14" t="s">
+      <c r="A89" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E89" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="13" t="s">
+      <c r="A91" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B91" s="11"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="13" t="s">
+      <c r="A92" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="11"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93" s="13"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
+      <c r="A93" s="12"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1579,24 +1624,395 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.88671875" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" style="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="27">
+        <v>1.0426989069530008</v>
+      </c>
+      <c r="C5" s="27">
+        <v>1.0255796080440631</v>
+      </c>
+      <c r="D5" s="27">
+        <v>1.0339467366576427</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+    </row>
+    <row r="6" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="28">
+        <v>1.790712718342661</v>
+      </c>
+      <c r="C7" s="28">
+        <v>1.383940722378858</v>
+      </c>
+      <c r="D7" s="28">
+        <v>1.5834018965271976</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="28">
+        <v>0.49387675765856898</v>
+      </c>
+      <c r="C8" s="28">
+        <v>0.34022115445313084</v>
+      </c>
+      <c r="D8" s="28">
+        <v>0.41556637815077124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="28">
+        <v>-0.2292073924337874</v>
+      </c>
+      <c r="C9" s="28">
+        <v>-0.20834525366782408</v>
+      </c>
+      <c r="D9" s="28">
+        <v>-0.21857503038498649</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0.1121911484176259</v>
+      </c>
+      <c r="C10" s="28">
+        <v>3.5209051270745917E-2</v>
+      </c>
+      <c r="D10" s="28">
+        <v>7.295732213913908E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="28">
+        <v>-0.26931024278284532</v>
+      </c>
+      <c r="C11" s="28">
+        <v>-0.21475326191479382</v>
+      </c>
+      <c r="D11" s="28">
+        <v>-0.24150534802176971</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="28">
+        <v>6.9854063885399498E-2</v>
+      </c>
+      <c r="C12" s="28">
+        <v>0.1580564774578761</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0.11480630992311625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="28">
+        <v>0.21943438920973612</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0.15848367800767527</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0.18837093805057314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="28">
+        <v>-0.1839322663329952</v>
+      </c>
+      <c r="C14" s="28">
+        <v>-0.1332215825171712</v>
+      </c>
+      <c r="D14" s="28">
+        <v>-0.15808763189159691</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="28">
+        <v>-5.533390346455036E-2</v>
+      </c>
+      <c r="C15" s="28">
+        <v>-6.3248404803601943E-3</v>
+      </c>
+      <c r="D15" s="28">
+        <v>-3.035649787991801E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="28">
+        <v>-2.3263432034053011E-3</v>
+      </c>
+      <c r="C16" s="28">
+        <v>-5.0659622644673163E-3</v>
+      </c>
+      <c r="D16" s="28">
+        <v>-3.7225865157406446E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="28">
+        <v>-0.15524621095374691</v>
+      </c>
+      <c r="C17" s="28">
+        <v>-0.12425946034481328</v>
+      </c>
+      <c r="D17" s="28">
+        <v>-0.13945385356958617</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="28">
+        <v>1.1419549588626206</v>
+      </c>
+      <c r="C19" s="28">
+        <v>0.81573513895701399</v>
+      </c>
+      <c r="D19" s="28">
+        <v>0.9500822595575551</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="28">
+        <v>0.75641068979665071</v>
+      </c>
+      <c r="C20" s="28">
+        <v>0.52687329662690807</v>
+      </c>
+      <c r="D20" s="28">
+        <v>0.63877466577115705</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="28">
+        <v>-0.30752596277633515</v>
+      </c>
+      <c r="C21" s="28">
+        <v>-0.23570846603234763</v>
+      </c>
+      <c r="D21" s="28">
+        <v>-0.2706953814434705</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="28">
+        <v>0.1203534800333923</v>
+      </c>
+      <c r="C22" s="28">
+        <v>6.2251856949341544E-2</v>
+      </c>
+      <c r="D22" s="28">
+        <v>9.0539420765750833E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="28">
+        <v>-0.38371867624212364</v>
+      </c>
+      <c r="C23" s="28">
+        <v>-0.29630408822661103</v>
+      </c>
+      <c r="D23" s="28">
+        <v>-0.33898888233904323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="28">
+        <v>-6.1824016155835437E-2</v>
+      </c>
+      <c r="C24" s="28">
+        <v>4.8186532312094243E-2</v>
+      </c>
+      <c r="D24" s="28">
+        <v>-5.4873214283759353E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="28">
+        <v>0.19115246263151242</v>
+      </c>
+      <c r="C25" s="28">
+        <v>8.4410067417714174E-2</v>
+      </c>
+      <c r="D25" s="28">
+        <v>0.13644786398416464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="28">
+        <v>-0.18861665194521215</v>
+      </c>
+      <c r="C26" s="28">
+        <v>-0.16357034731018771</v>
+      </c>
+      <c r="D26" s="28">
+        <v>-0.17577201099042661</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="28">
+        <v>-0.13916894378140832</v>
+      </c>
+      <c r="C27" s="28">
+        <v>-8.9110184283535787E-2</v>
+      </c>
+      <c r="D27" s="28">
+        <v>-0.11348197079658817</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="28">
+        <v>4.3080785005368938E-2</v>
+      </c>
+      <c r="C28" s="28">
+        <v>3.8633807211086335E-2</v>
+      </c>
+      <c r="D28" s="28">
+        <v>4.0805279226006519E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="28">
+        <v>-9.2058249357402033E-2</v>
+      </c>
+      <c r="C29" s="28">
+        <v>-8.642163154420146E-2</v>
+      </c>
+      <c r="D29" s="28">
+        <v>-8.9171722370126716E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>